<commit_message>
Updated and added files
</commit_message>
<xml_diff>
--- a/LeetCode_150_Quest.xlsx
+++ b/LeetCode_150_Quest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57188cc0fe39b4ad/Desktop/Coding_Programming/LeetCode Problems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_706521920712BF640C1BC786C343BACE75F71A7C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D5D469A-2A13-42AD-B641-2628BEC2B59C}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_12D1959B44054B14032F2F312800A9B274F7F909" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14F0A511-95E0-4E39-9B90-CC54E91D7A43}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leetcode_Quest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>Number</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Kth Largest Element in a Stream</t>
-  </si>
-  <si>
-    <t>INCOMPLETE</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/kth-largest-element-in-a-stream/</t>
@@ -195,6 +192,9 @@
     <t>Number of Islands</t>
   </si>
   <si>
+    <t>INCOMPLETE</t>
+  </si>
+  <si>
     <t>https://leetcode.com/problems/number-of-islands/</t>
   </si>
   <si>
@@ -207,12 +207,27 @@
     <t>https://leetcode.com/problems/valid-palindrome/</t>
   </si>
   <si>
+    <t>To understand and solve this problem you need to first make sure that the values being compared are lowercase and to remove non alphanumeric 
+characters from the string. Ideally in Solution1 and Solution3 we create pointers to compare the beginining of a string to the end of the string and if the 
+values are equal all through the iteration of the string then it is a valid palindrome. If any value is different then it is not a valid palindrome. There are 
+many ways to acheive this you can use regular expression, python built in string functions, or create a helper function that will check if each value in the string 
+is alphanumeric.</t>
+  </si>
+  <si>
     <t>Two Sum</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/two-sum/</t>
   </si>
   <si>
+    <t>To understand and solve this problem you can use different solutions. The slower solution involves the brute force method which requires two for loops 
+to run through the array of numbers and compare each value pair in the array to see if it equals the target. If it does then it will return the index of it. The next 
+more optimal method is using a hashmap that will take in as it key the value of the element in the array and as it's value it will take in the index of the integer in 
+the array. For this you will only need to iterate through the array once and use the enumerate function to keep track of the index and values in the array. You will 
+also need to keep track of the difference which is the target - integer value. You would check to see if the difference is not in the hashtable; if not append the 
+integer value as the key and the index as the value. If the difference is in the hashmap then we just return the index of the hashmap[difference] and i in a list.</t>
+  </si>
+  <si>
     <t>Sliding Window</t>
   </si>
   <si>
@@ -222,13 +237,36 @@
     <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/</t>
   </si>
   <si>
+    <t>To understand and solve this problem it is best to solve this by using two pointers. Use one pointer to be 0 and the other pointer to be 1. Create a 
+variable to equal maxprofit to hold the max numbers. You can use a while loop that will iterate as long as bigger pointer is less than the length of the array. You 
+then check if the value of lower pointer in the index is less than the value of the higher pointer in the index. If it is then calculate the profit by subtracting 
+values from the array that correspond with the lower pointer and the higher pointer than update maxP to equal the max of maxP and the profit. If the lower index value 
+is greater than the higher index value make the lower index equal the higher index and increment the higher index +1. Finally return maxP</t>
+  </si>
+  <si>
     <t>Min Stack</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/min-stack/</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>To understand and solve this problem you need to pretty much implement a min stack. A min stack pretty much is a regular stack except the min number in 
+the stack is on the top. This one is tricky because you have to retrieve the min number in the stack in constant time which is O(1) time. The min function uses O(n) 
+time because it's iterating over the stack. So the big takeaway with this is create another list called min stack in the init function of the class. Append the min 
+value and compare the current value being appended and the value at index[-1] of the minstack. If the minStack is empty it will just append the value to the min stack. 
+Otherwise it will compare both values. For the function which says return min number you just return the number at index [-1] in the min stack.</t>
+  </si>
+  <si>
+    <t>Diameter of a Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/diameter-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>Maximum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-depth-of-binary-tree/</t>
   </si>
 </sst>
 </file>
@@ -603,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +655,7 @@
     <col min="4" max="4" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5546875" customWidth="1"/>
     <col min="6" max="6" width="61.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="79.109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -643,7 +681,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -666,7 +704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -689,7 +727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -712,7 +750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -735,7 +773,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="158.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -758,7 +796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -775,79 +813,79 @@
         <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:7" ht="230.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -855,22 +893,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>42</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>43</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -884,13 +922,16 @@
         <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -901,36 +942,42 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -941,19 +988,59 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F18" t="s">
-        <v>55</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F6" xr:uid="{00000000-0009-0000-0000-000000000000}">
@@ -967,6 +1054,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>